<commit_message>
[METH] Set up Final MS Word Document
</commit_message>
<xml_diff>
--- a/resources/Imagens_Diagramas_Tabelas.xlsx
+++ b/resources/Imagens_Diagramas_Tabelas.xlsx
@@ -264,7 +264,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>152120</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
@@ -276,15 +276,15 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="22" name="Grupo 21"/>
+        <xdr:cNvPr id="16" name="Grupo 15"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1324535" y="590550"/>
-          <a:ext cx="6665819" cy="4610100"/>
-          <a:chOff x="1333500" y="590550"/>
-          <a:chExt cx="6715125" cy="4610100"/>
+          <a:off x="1362355" y="590550"/>
+          <a:ext cx="6627999" cy="4610100"/>
+          <a:chOff x="1362355" y="590550"/>
+          <a:chExt cx="6627999" cy="4610100"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -294,18 +294,13 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1371600" y="590550"/>
-            <a:ext cx="6619875" cy="3648075"/>
+            <a:off x="1362355" y="590550"/>
+            <a:ext cx="6571268" cy="3648075"/>
           </a:xfrm>
           <a:prstGeom prst="triangle">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-              <a:alpha val="38000"/>
-            </a:schemeClr>
-          </a:solidFill>
+          <a:noFill/>
           <a:ln>
             <a:solidFill>
               <a:schemeClr val="tx1">
@@ -313,6 +308,7 @@
                 <a:lumOff val="50000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="dash"/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
@@ -336,412 +332,455 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="pt-BR" sz="1100"/>
+            <a:endParaRPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="8" name="Conector reto 7"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="3" idx="0"/>
-            <a:endCxn id="2" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="4662488" y="590550"/>
-            <a:ext cx="19050" cy="2238375"/>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="14" name="Grupo 13"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1381265" y="590550"/>
+            <a:ext cx="6609089" cy="4610100"/>
+            <a:chOff x="1381265" y="590550"/>
+            <a:chExt cx="6609089" cy="4610100"/>
           </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="44450">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Triângulo isósceles 2"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1333500" y="2828925"/>
-            <a:ext cx="6657975" cy="1381125"/>
-          </a:xfrm>
-          <a:prstGeom prst="triangle">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="44450">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="pt-BR" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="CaixaDeTexto 10"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1476375" y="1104899"/>
-            <a:ext cx="3105151" cy="1228726"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="8" name="Conector reto 7"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="3" idx="0"/>
+              <a:endCxn id="2" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="4639236" y="590550"/>
+              <a:ext cx="8753" cy="2238375"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="44450">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Triângulo isósceles 2"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1423147" y="2828925"/>
+              <a:ext cx="6432177" cy="1381125"/>
+            </a:xfrm>
+            <a:prstGeom prst="triangle">
+              <a:avLst/>
+            </a:prstGeom>
             <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1">
+            <a:ln w="44450">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:endParaRPr lang="pt-BR" sz="1100">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="CaixaDeTexto 10"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1466361" y="1104899"/>
+              <a:ext cx="3082351" cy="1228726"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Capacidade:</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Capacidade:</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1200" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="2200" b="1" baseline="0">
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="2000" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Manutenção </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>e Teste</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Flexibilidade</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1400" b="1">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Manutenção</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> e Teste</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Flexibilidade</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="CaixaDeTexto 11"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5495925" y="1123950"/>
-            <a:ext cx="2219325" cy="1038226"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Portabilidade</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="2200" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Reusabilidade</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Interoperabilidade</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="CaixaDeTexto 14"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1390650" y="4238624"/>
-            <a:ext cx="6657975" cy="962026"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Acurácia 			Confiabilidade		E</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>ficiência</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>	</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="2200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Usabilidade 			</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Integridade</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="CaixaDeTexto 11"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5456397" y="1123950"/>
+              <a:ext cx="2203030" cy="1038226"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Portabilidade</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="2200" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Reusabilidade</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="r"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Interoperabilidade</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="CaixaDeTexto 14"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1381265" y="4238624"/>
+              <a:ext cx="6609089" cy="962026"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Acurácia 			Confiabilidade		E</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1600" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>ficiência</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>	</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="2800" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Usabilidade </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="2200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>			</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Integridade</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -752,10 +791,93 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3286125" y="666751"/>
+          <a:ext cx="2181225" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+              <a:alpha val="55000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>PORTABILIDADE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -765,15 +887,15 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="34" name="Grupo 33"/>
+        <xdr:cNvPr id="22" name="Grupo 21"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2057400" y="666751"/>
-          <a:ext cx="8048625" cy="4333875"/>
-          <a:chOff x="2057400" y="666751"/>
-          <a:chExt cx="8048625" cy="4333875"/>
+          <a:off x="2057400" y="695326"/>
+          <a:ext cx="8048625" cy="4305300"/>
+          <a:chOff x="2057400" y="695326"/>
+          <a:chExt cx="8048625" cy="4305300"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -793,8 +915,17 @@
             <a:schemeClr val="tx1">
               <a:lumMod val="65000"/>
               <a:lumOff val="35000"/>
+              <a:alpha val="53000"/>
             </a:schemeClr>
           </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -818,7 +949,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1600">
+              <a:rPr lang="pt-BR" sz="1400" b="1">
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
@@ -827,7 +958,7 @@
           </a:p>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="pt-BR" sz="900">
+            <a:endParaRPr lang="pt-BR" sz="1400" b="1">
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:endParaRPr>
@@ -835,20 +966,20 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1100">
+              <a:rPr lang="pt-BR" sz="1400" b="1">
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Qualidade</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1100" baseline="0">
+              <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t> do Produto</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1100">
+            <a:endParaRPr lang="pt-BR" sz="1400" b="1">
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:endParaRPr>
@@ -870,8 +1001,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -937,8 +1068,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1005,8 +1136,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1073,8 +1204,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1128,74 +1259,6 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3286125" y="666751"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>PORTABILIDADE</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
           <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
@@ -1209,8 +1272,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1277,8 +1340,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1345,8 +1408,8 @@
           </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-              <a:alpha val="45000"/>
+              <a:lumMod val="75000"/>
+              <a:alpha val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:ln>
@@ -1608,13 +1671,13 @@
           <xdr:cNvPr id="24" name="Conector reto 23"/>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="2" idx="1"/>
-            <a:endCxn id="10" idx="0"/>
+            <a:endCxn id="10" idx="3"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1">
-            <a:off x="3148013" y="2847976"/>
-            <a:ext cx="1852613" cy="495300"/>
+            <a:off x="4238625" y="2847976"/>
+            <a:ext cx="762001" cy="809625"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -1738,14 +1801,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1754,10 +1817,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1247775" y="38100"/>
-          <a:ext cx="6362699" cy="3562350"/>
-          <a:chOff x="1247775" y="38100"/>
-          <a:chExt cx="6362699" cy="3562350"/>
+          <a:off x="1247775" y="247650"/>
+          <a:ext cx="6448425" cy="3648075"/>
+          <a:chOff x="1247775" y="-47625"/>
+          <a:chExt cx="6448425" cy="3648075"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -2502,11 +2565,11 @@
           <a:p>
             <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+              <a:rPr lang="pt-BR" sz="1200" b="1" u="none">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
@@ -2516,11 +2579,11 @@
           <a:p>
             <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+              <a:rPr lang="pt-BR" sz="1200" b="1" u="none">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
@@ -2575,7 +2638,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3495675" y="2257424"/>
+            <a:off x="3495675" y="2266949"/>
             <a:ext cx="2552700" cy="619125"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2608,8 +2671,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1200" b="1" u="none">
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
@@ -2619,8 +2682,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1200" b="1" u="none" baseline="0">
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
@@ -2673,8 +2736,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4229100" y="1543049"/>
-            <a:ext cx="2476500" cy="752476"/>
+            <a:off x="4286249" y="1600199"/>
+            <a:ext cx="3409951" cy="809626"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2706,15 +2769,15 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Processo de software para gestão e desenvolvimento é documentado, padronizado e integrado em um processo global para a organização</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
-              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="1" u="none" baseline="0">
+              <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
               <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
               <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
             </a:endParaRPr>
@@ -2796,20 +2859,18 @@
           <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="l"/>
+            <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Processos e produtos são quantitativamente compreendidos e controlados</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
-              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2857,7 +2918,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5448299" y="38100"/>
+            <a:off x="5524499" y="-47625"/>
             <a:ext cx="2162175" cy="752476"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -2888,20 +2949,18 @@
           <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="l"/>
+            <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
-                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Melhoria contínua dos processos através de feedback quantitativo</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
-              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -3236,7 +3295,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3251,7 +3310,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M14" activeCellId="1" sqref="N15 M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3524,7 +3583,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[METH] Initial Steps/ Review and Fix issues
</commit_message>
<xml_diff>
--- a/resources/Imagens_Diagramas_Tabelas.xlsx
+++ b/resources/Imagens_Diagramas_Tabelas.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
+    <sheet name="Plan4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Nível</t>
   </si>
@@ -158,13 +159,140 @@
   </si>
   <si>
     <t>- Gestão de Desempenho Organizacional</t>
+  </si>
+  <si>
+    <t>Normas e Modelos existentes na área de Qualidade</t>
+  </si>
+  <si>
+    <t>Norma/Modelo</t>
+  </si>
+  <si>
+    <t>ISO/IEC 9126</t>
+  </si>
+  <si>
+    <t>Define as características de qualidade referentes aos produtos de</t>
+  </si>
+  <si>
+    <t>software.</t>
+  </si>
+  <si>
+    <t>NBR 13596</t>
+  </si>
+  <si>
+    <t>Versão brasileira da norma ISO/IEC 9126. Avaliação do produto de</t>
+  </si>
+  <si>
+    <t>software – características de qualidade e diretrizes para o seu uso.</t>
+  </si>
+  <si>
+    <t>ISO 14598</t>
+  </si>
+  <si>
+    <t>Guias para a avaliação de produtos de software, baseados na utilização</t>
+  </si>
+  <si>
+    <t>prática da norma ISO 9126.</t>
+  </si>
+  <si>
+    <t>ISO/IEC 12119</t>
+  </si>
+  <si>
+    <t>Esta norma estabelece os requisitos para pacotes de software (requisitos</t>
+  </si>
+  <si>
+    <t>de qualidade), instruções de como testar um pacote de software com</t>
+  </si>
+  <si>
+    <t>relação aos requisitos estabelecidos.</t>
+  </si>
+  <si>
+    <t>Estabelece processos, atividades e tarefas a serem executadas durante os</t>
+  </si>
+  <si>
+    <t>processos de aquisição, fornecimento, operação, desenvolvimento e</t>
+  </si>
+  <si>
+    <t>manutenção de software.</t>
+  </si>
+  <si>
+    <t>NBR ISO 9001</t>
+  </si>
+  <si>
+    <t>Sistemas de qualidade – Modelo para garantia de qualidade em Projeto,</t>
+  </si>
+  <si>
+    <t>Desenvolvimento, Instalação e Assistência Técnica (processo).</t>
+  </si>
+  <si>
+    <t>NBR ISO 9000-3</t>
+  </si>
+  <si>
+    <t>Define diretrizes para facilitar a aplicação da NBR ISO 9001 em</t>
+  </si>
+  <si>
+    <t>organizações que desenvolvem, fornecem e mantêm software.</t>
+  </si>
+  <si>
+    <t>ISSO/IEC 15504</t>
+  </si>
+  <si>
+    <t>Avalia o processo de software, visando orientar a organização na busca</t>
+  </si>
+  <si>
+    <t>pela melhoria contínua do processo.</t>
+  </si>
+  <si>
+    <t>CMM</t>
+  </si>
+  <si>
+    <t>Tem como objetivo avaliar e melhorar a capacitação das empresas que</t>
+  </si>
+  <si>
+    <t>produzem software. Neste modelo, a área de processo responsável pela</t>
+  </si>
+  <si>
+    <t>qualidade é SQA.</t>
+  </si>
+  <si>
+    <t>CMMI</t>
+  </si>
+  <si>
+    <t>Elaborado para integrar os diferentes modelos criados a partir do CMM.</t>
+  </si>
+  <si>
+    <t>O modelo CMMI introduziu 2 representações para apresentar seu</t>
+  </si>
+  <si>
+    <t>conteúdo. A área de processo responsável pela qualidade é a Garantia da</t>
+  </si>
+  <si>
+    <t>Qualidade de Processo e de Produto.</t>
+  </si>
+  <si>
+    <t>MPS.BR</t>
+  </si>
+  <si>
+    <t>É um modelo de melhoria e avaliação de processo de software,</t>
+  </si>
+  <si>
+    <t>preferencialmente voltado para as micro, pequenas e médias empresas, de</t>
+  </si>
+  <si>
+    <t>forma a atender as suas necessidades de negócio.</t>
+  </si>
+  <si>
+    <t>Fonte: Adaptado de Barreto Jr. (2001).</t>
+  </si>
+  <si>
+    <t>ISO/IEC 12207 
+Revisada pela ISO/IEC 25010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +309,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -206,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,11 +373,19 @@
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,93 +939,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3286125" y="666751"/>
-          <a:ext cx="2181225" cy="628650"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="75000"/>
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-              <a:alpha val="55000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>PORTABILIDADE</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -887,180 +952,25 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="22" name="Grupo 21"/>
+        <xdr:cNvPr id="20" name="Grupo 19"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2057400" y="695326"/>
-          <a:ext cx="8048625" cy="4305300"/>
-          <a:chOff x="2057400" y="695326"/>
-          <a:chExt cx="8048625" cy="4305300"/>
+          <a:off x="2057400" y="666751"/>
+          <a:ext cx="8048625" cy="4333875"/>
+          <a:chOff x="2057400" y="666751"/>
+          <a:chExt cx="8048625" cy="4333875"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1"/>
+          <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5000626" y="2352675"/>
-            <a:ext cx="2190750" cy="990601"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-              <a:alpha val="53000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400" b="1">
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>ISO/IEC 25010:2011</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="pt-BR" sz="1400" b="1">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400" b="1">
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Qualidade</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> do Produto</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1400" b="1">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Retângulo de cantos arredondados 2"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6705600" y="695326"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>FUNCIONALIDADE</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Retângulo de cantos arredondados 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7924800" y="1714501"/>
+            <a:off x="3286125" y="666751"/>
             <a:ext cx="2181225" cy="628650"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -1116,679 +1026,916 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>CONFIABILIDADE</a:t>
+              <a:t>PORTABILIDADE</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Retângulo de cantos arredondados 4"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="22" name="Grupo 21"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="7924800" y="3343276"/>
-            <a:ext cx="2181225" cy="628650"/>
+            <a:off x="2057400" y="695326"/>
+            <a:ext cx="8048625" cy="4305300"/>
+            <a:chOff x="2057400" y="695326"/>
+            <a:chExt cx="8048625" cy="4305300"/>
           </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5000626" y="2352675"/>
+              <a:ext cx="2190750" cy="990601"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="53000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1">
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>ISO/IEC 25010:2011</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:endParaRPr lang="pt-BR" sz="1400" b="1">
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>OPERABILIDADE</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Retângulo de cantos arredondados 5"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6705600" y="4371976"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1">
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Qualidade</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t> do Produto</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1400" b="1">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Retângulo de cantos arredondados 2"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6705600" y="695326"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>SEGURANÇA</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3286125" y="4343401"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>FUNCIONALIDADE</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="Retângulo de cantos arredondados 3"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7924800" y="1714501"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>COMPATIBILIDADE</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2057400" y="1714501"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>CONFIABILIDADE</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Retângulo de cantos arredondados 4"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7924800" y="3343276"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>CAPACIDADE DE MANUTENÇÃO</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Retângulo de cantos arredondados 9"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2057400" y="3343276"/>
-            <a:ext cx="2181225" cy="628650"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>OPERABILIDADE</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Retângulo de cantos arredondados 5"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6705600" y="4371976"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="55000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1400">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>EFICIÊNCIA</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="Conector reto 11"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="3"/>
-            <a:endCxn id="3" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="7191376" y="1323976"/>
-            <a:ext cx="604837" cy="1524000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>SEGURANÇA</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3286125" y="4343401"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="14" name="Conector reto 13"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="3"/>
-            <a:endCxn id="4" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="7191376" y="2028826"/>
-            <a:ext cx="733424" cy="819150"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>COMPATIBILIDADE</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2057400" y="1714501"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="17" name="Conector reto 16"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="3"/>
-            <a:endCxn id="5" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7191376" y="2847976"/>
-            <a:ext cx="733424" cy="809625"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>CAPACIDADE DE MANUTENÇÃO</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Retângulo de cantos arredondados 9"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2057400" y="3343276"/>
+              <a:ext cx="2181225" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="18" name="Conector reto 17"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="3"/>
-            <a:endCxn id="6" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7191376" y="2847976"/>
-            <a:ext cx="604837" cy="1524000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="21" name="Conector reto 20"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="1"/>
-            <a:endCxn id="8" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="4376738" y="2847976"/>
-            <a:ext cx="623888" cy="1495425"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="24" name="Conector reto 23"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="1"/>
-            <a:endCxn id="10" idx="3"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="4238625" y="2847976"/>
-            <a:ext cx="762001" cy="809625"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="27" name="Conector reto 26"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="1"/>
-            <a:endCxn id="9" idx="3"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="4238625" y="2028826"/>
-            <a:ext cx="762001" cy="819150"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="30" name="Conector reto 29"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="1"/>
-            <a:endCxn id="7" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="4376738" y="1295401"/>
-            <a:ext cx="623888" cy="1552575"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="sysDot"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>EFICIÊNCIA</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="12" name="Conector reto 11"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="3"/>
+              <a:endCxn id="3" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="7191376" y="1323976"/>
+              <a:ext cx="604837" cy="1524000"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="14" name="Conector reto 13"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="3"/>
+              <a:endCxn id="4" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="7191376" y="2028826"/>
+              <a:ext cx="733424" cy="819150"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="17" name="Conector reto 16"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="3"/>
+              <a:endCxn id="5" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7191376" y="2847976"/>
+              <a:ext cx="733424" cy="809625"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="18" name="Conector reto 17"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="3"/>
+              <a:endCxn id="6" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7191376" y="2847976"/>
+              <a:ext cx="604837" cy="1524000"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="21" name="Conector reto 20"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="1"/>
+              <a:endCxn id="8" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="4376738" y="2847976"/>
+              <a:ext cx="623888" cy="1495425"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="24" name="Conector reto 23"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="1"/>
+              <a:endCxn id="10" idx="3"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="4238625" y="2847976"/>
+              <a:ext cx="762001" cy="809625"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="27" name="Conector reto 26"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="1"/>
+              <a:endCxn id="9" idx="3"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1" flipV="1">
+              <a:off x="4238625" y="2028826"/>
+              <a:ext cx="762001" cy="819150"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="30" name="Conector reto 29"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="1"/>
+              <a:endCxn id="7" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1" flipV="1">
+              <a:off x="4376738" y="1295401"/>
+              <a:ext cx="623888" cy="1552575"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1802,11 +1949,11 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -1817,10 +1964,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1247775" y="247650"/>
-          <a:ext cx="6448425" cy="3648075"/>
-          <a:chOff x="1247775" y="-47625"/>
-          <a:chExt cx="6448425" cy="3648075"/>
+          <a:off x="1247775" y="323850"/>
+          <a:ext cx="6591300" cy="3571875"/>
+          <a:chOff x="1247775" y="28575"/>
+          <a:chExt cx="6591300" cy="3571875"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -2569,9 +2716,9 @@
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Ad Hoc, Ocasionalmente caótico</a:t>
             </a:r>
@@ -2583,9 +2730,9 @@
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Poucos processos definidos</a:t>
             </a:r>
@@ -2638,198 +2785,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3495675" y="2266949"/>
-            <a:ext cx="2552700" cy="619125"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" u="none">
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Gerenciamento básico dos projetos.</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1200" b="1" u="none" baseline="0">
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>(Custo, Cronograma, Prazo)</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="34" name="Conector reto 33"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3486150" y="2562225"/>
-            <a:ext cx="609600" cy="1"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="CaixaDeTexto 34"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4286249" y="1600199"/>
-            <a:ext cx="3409951" cy="809626"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Processo de software para gestão e desenvolvimento é documentado, padronizado e integrado em um processo global para a organização</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1100" b="1" u="none" baseline="0">
-              <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="36" name="Conector reto 35"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4067175" y="1914525"/>
-            <a:ext cx="609600" cy="1"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="CaixaDeTexto 36"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4952999" y="838199"/>
-            <a:ext cx="2162175" cy="752476"/>
+            <a:off x="3667125" y="2314574"/>
+            <a:ext cx="3200400" cy="504826"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2865,23 +2822,37 @@
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Processos e produtos são quantitativamente compreendidos e controlados</a:t>
+              <a:t>Gerenciamento básico dos projetos.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>(Custo, Cronograma, Prazo)</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="38" name="Conector reto 37"/>
+          <xdr:cNvPr id="34" name="Conector reto 33"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4705350" y="1143000"/>
+            <a:off x="3486150" y="2562225"/>
             <a:ext cx="609600" cy="1"/>
           </a:xfrm>
           <a:prstGeom prst="line">
@@ -2913,13 +2884,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="39" name="CaixaDeTexto 38"/>
+          <xdr:cNvPr id="35" name="CaixaDeTexto 34"/>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5524499" y="-47625"/>
-            <a:ext cx="2162175" cy="752476"/>
+            <a:off x="4362449" y="1514474"/>
+            <a:ext cx="3409951" cy="809626"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2955,9 +2926,189 @@
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Segoe UI Light" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Processo de software para gestão e desenvolvimento é documentado, padronizado e integrado em um processo global para a organização</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="36" name="Conector reto 35"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4067175" y="1914525"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="CaixaDeTexto 36"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4952999" y="838199"/>
+            <a:ext cx="2600326" cy="752476"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Processos e produtos são quantitativamente compreendidos e controlados</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="38" name="Conector reto 37"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4705350" y="1143000"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="CaixaDeTexto 38"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5524499" y="28575"/>
+            <a:ext cx="2314576" cy="752476"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Melhoria contínua dos processos através de feedback quantitativo</a:t>
             </a:r>
@@ -3309,9 +3460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="M14" activeCellId="1" sqref="N15 M14"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -3321,6 +3470,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -3347,7 +3511,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="10">
+      <c r="A2" s="13">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3358,7 +3522,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3367,7 +3531,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -3376,7 +3540,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3385,7 +3549,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -3394,7 +3558,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3403,7 +3567,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -3417,7 +3581,7 @@
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="10">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3428,7 +3592,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
@@ -3437,7 +3601,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
@@ -3446,7 +3610,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3455,7 +3619,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
@@ -3464,7 +3628,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
@@ -3473,7 +3637,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
@@ -3482,7 +3646,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
@@ -3491,7 +3655,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
@@ -3500,7 +3664,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
@@ -3509,7 +3673,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="10"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
@@ -3523,7 +3687,7 @@
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="11">
+      <c r="A22" s="14">
         <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3534,7 +3698,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="11"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="7" t="s">
         <v>41</v>
       </c>
@@ -3548,7 +3712,7 @@
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" ht="15.75">
-      <c r="A25" s="11">
+      <c r="A25" s="14">
         <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3559,7 +3723,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75">
-      <c r="A26" s="11"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="7" t="s">
         <v>45</v>
       </c>
@@ -3578,17 +3742,218 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="39" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.5">
+      <c r="A11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[METH] Initial steps Methodology Chapter
</commit_message>
<xml_diff>
--- a/resources/Imagens_Diagramas_Tabelas.xlsx
+++ b/resources/Imagens_Diagramas_Tabelas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Plan3" sheetId="3" r:id="rId4"/>
     <sheet name="Plan4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -291,8 +292,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1059,9 +1060,9 @@
             </a:prstGeom>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="53000"/>
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+                <a:alpha val="64000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -3158,10 +3159,886 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="1123950"/>
+          <a:ext cx="1685925" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Objetivos</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="1600201"/>
+          <a:ext cx="1285876" cy="781049"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SG</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="3038476"/>
+          <a:ext cx="1285876" cy="781049"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SG 2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705226" y="2276476"/>
+          <a:ext cx="1152523" cy="552449"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SP 1.2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695701" y="1590676"/>
+          <a:ext cx="1152523" cy="552449"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SP 1.1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695701" y="3543301"/>
+          <a:ext cx="1152523" cy="552449"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SP 2.2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Oval 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3686176" y="2895601"/>
+          <a:ext cx="1152523" cy="552449"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SP 2.1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rectangle 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3076575" y="1057275"/>
+          <a:ext cx="2305050" cy="3209925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Práticas</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2543176" y="1866901"/>
+          <a:ext cx="1152525" cy="123825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2543176" y="1990726"/>
+          <a:ext cx="1162050" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2524126" y="3171826"/>
+          <a:ext cx="1162050" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524126" y="3429001"/>
+          <a:ext cx="1171575" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3199,7 +4076,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3233,6 +4110,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3267,9 +4145,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3442,14 +4321,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3457,12 +4336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3470,14 +4351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3485,21 +4366,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3510,7 +4391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>2</v>
       </c>
@@ -3521,7 +4402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -3530,7 +4411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -3539,7 +4420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -3548,7 +4429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -3557,7 +4438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -3566,7 +4447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -3575,12 +4456,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>3</v>
       </c>
@@ -3591,7 +4472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="4" t="s">
         <v>19</v>
@@ -3600,7 +4481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
         <v>21</v>
@@ -3609,7 +4490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
@@ -3618,7 +4499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -3627,7 +4508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -3636,7 +4517,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>29</v>
@@ -3645,7 +4526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
@@ -3654,7 +4535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="4" t="s">
         <v>33</v>
@@ -3663,7 +4544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -3672,7 +4553,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>37</v>
@@ -3681,12 +4562,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>4</v>
       </c>
@@ -3697,7 +4578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="7" t="s">
         <v>41</v>
@@ -3706,12 +4587,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>5</v>
       </c>
@@ -3722,7 +4603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="7" t="s">
         <v>45</v>
@@ -3743,27 +4624,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
@@ -3771,7 +4652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
@@ -3779,12 +4660,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -3792,12 +4673,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>55</v>
       </c>
@@ -3805,12 +4686,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>58</v>
       </c>
@@ -3818,12 +4699,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.5">
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -3831,22 +4712,22 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>65</v>
       </c>
@@ -3854,12 +4735,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>68</v>
       </c>
@@ -3867,12 +4748,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>71</v>
       </c>
@@ -3880,12 +4761,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>74</v>
       </c>
@@ -3893,17 +4774,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>78</v>
       </c>
@@ -3911,22 +4792,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>83</v>
       </c>
@@ -3934,17 +4815,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>87</v>
       </c>
@@ -3956,4 +4837,19 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[METH] Methodology and Conclusion development/sent
</commit_message>
<xml_diff>
--- a/resources/Imagens_Diagramas_Tabelas.xlsx
+++ b/resources/Imagens_Diagramas_Tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Plan3" sheetId="3" r:id="rId4"/>
     <sheet name="Plan4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="Plan5" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>Nível</t>
   </si>
@@ -286,13 +288,64 @@
   <si>
     <t>ISO/IEC 12207 
 Revisada pela ISO/IEC 25010</t>
+  </si>
+  <si>
+    <t>SP 1.1 Avaliar objetivamente processos realizados selecionado contra descrições aplicáveis processo, padrões e procedimentos.</t>
+  </si>
+  <si>
+    <t>SP 1.2 Avaliar objetivamente produtos de trabalho selecionado contra as descrições aplicáveis processo, padrões e procedimentos.</t>
+  </si>
+  <si>
+    <t>SP 2.1 Comunicar problemas de qualidade e garantir a resolução dos problemas de não conformidade com a equipe e gestores.</t>
+  </si>
+  <si>
+    <t>SP 2.2 Estabelecer e manter registros das atividades de garantia de qualidade.</t>
+  </si>
+  <si>
+    <t>CMMI-DEV - PPQA</t>
+  </si>
+  <si>
+    <t>Abordagem proposta</t>
+  </si>
+  <si>
+    <t>Extra - Atividades de Suporte e informativas</t>
+  </si>
+  <si>
+    <t>Aderência do método proposto</t>
+  </si>
+  <si>
+    <t>3.    Avaliar objetivamente os processos</t>
+  </si>
+  <si>
+    <t>2.    Avaliar objetivamente os produtos de trabalho e serviços</t>
+  </si>
+  <si>
+    <t>4.    Aprovar produto final para entrega</t>
+  </si>
+  <si>
+    <t>6.    Elaborar relatório de não conformidades</t>
+  </si>
+  <si>
+    <t>1.    Elaborar plano de qualidade</t>
+  </si>
+  <si>
+    <t>5.    Elaborar relatório periódico de garantia da qualidade</t>
+  </si>
+  <si>
+    <t>7.    Elaborar relatório de lições aprendidas do projeto</t>
+  </si>
+  <si>
+    <t>8.    Disponibilizar materiais de treinamento para os integrantes do projeto</t>
+  </si>
+  <si>
+    <t>9.    Prestar suporte a todos os envolvidos no projeto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +378,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -346,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -378,6 +444,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,6 +470,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,9 +1146,9 @@
             </a:prstGeom>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="53000"/>
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+                <a:alpha val="64000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -3135,6 +3222,731 @@
                 <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="14" name="Grupo 13"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1047750" y="1057275"/>
+          <a:ext cx="4333875" cy="3209925"/>
+          <a:chOff x="1047750" y="1057275"/>
+          <a:chExt cx="4333875" cy="3209925"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Oval 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1047750" y="1123950"/>
+            <a:ext cx="1685925" cy="3095625"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Objetivos</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Oval 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1257300" y="1600201"/>
+            <a:ext cx="1285876" cy="781049"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2400" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SG</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Oval 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1238250" y="3038476"/>
+            <a:ext cx="1285876" cy="781049"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2400" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SG 2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Oval 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3705226" y="2276476"/>
+            <a:ext cx="1152523" cy="552449"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SP 1.2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Oval 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3695701" y="1590676"/>
+            <a:ext cx="1152523" cy="552449"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SP 1.1</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Oval 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3695701" y="3543301"/>
+            <a:ext cx="1152523" cy="552449"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SP 2.2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Oval 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3686176" y="2895601"/>
+            <a:ext cx="1152523" cy="552449"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SP 2.1</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="27" name="Rectangle 26"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3076575" y="1057275"/>
+            <a:ext cx="2305050" cy="3209925"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Práticas</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="39" name="Straight Arrow Connector 38"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="6"/>
+            <a:endCxn id="7" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2543176" y="1866901"/>
+            <a:ext cx="1152525" cy="123825"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="44450">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="6"/>
+            <a:endCxn id="6" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2543176" y="1990726"/>
+            <a:ext cx="1162050" cy="561975"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="44450">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="44" name="Straight Arrow Connector 43"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="6"/>
+            <a:endCxn id="9" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2524126" y="3171826"/>
+            <a:ext cx="1162050" cy="257175"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="44450">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="47" name="Straight Arrow Connector 46"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="6"/>
+            <a:endCxn id="8" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2524126" y="3429001"/>
+            <a:ext cx="1171575" cy="390525"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="44450">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
@@ -3460,7 +4272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -3511,7 +4325,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13">
+      <c r="A2" s="19">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3522,7 +4336,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3531,7 +4345,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -3540,7 +4354,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3549,7 +4363,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -3558,7 +4372,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3567,7 +4381,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -3581,7 +4395,7 @@
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="13">
+      <c r="A10" s="19">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3592,7 +4406,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
@@ -3601,7 +4415,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
@@ -3610,7 +4424,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3619,7 +4433,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
@@ -3628,7 +4442,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
@@ -3637,7 +4451,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
@@ -3646,7 +4460,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
@@ -3655,7 +4469,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
@@ -3664,7 +4478,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
@@ -3673,7 +4487,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
@@ -3687,7 +4501,7 @@
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="14">
+      <c r="A22" s="20">
         <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3698,7 +4512,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="14"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="7" t="s">
         <v>41</v>
       </c>
@@ -3712,7 +4526,7 @@
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" ht="15.75">
-      <c r="A25" s="14">
+      <c r="A25" s="20">
         <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3723,7 +4537,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75">
-      <c r="A26" s="14"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="7" t="s">
         <v>45</v>
       </c>
@@ -3758,10 +4572,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
@@ -3956,4 +4770,129 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" activeCellId="1" sqref="D7 F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="65.28515625" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" style="15"/>
+    <col min="4" max="16384" width="65.28515625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="48" customHeight="1">
+      <c r="A1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" ht="41.25" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="54">
+      <c r="A3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="54">
+      <c r="A4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" ht="40.5">
+      <c r="A5" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="21.75" customHeight="1">
+      <c r="A6" s="18"/>
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" ht="27">
+      <c r="A8" s="22"/>
+      <c r="B8" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27">
+      <c r="A9" s="22"/>
+      <c r="B9" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27">
+      <c r="A10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27">
+      <c r="A11" s="22"/>
+      <c r="B11" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>